<commit_message>
modificación de casoss de uso y mockups de caso de uso 3 y 4
Se modifica la descripción del caso de uso 04-generar proximos pagos de alumnos, asi como los mosckups de los casos de uso 3(generar recibo de pago) y 4
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla de Casos de Uso.xlsx
+++ b/Plantillas/Plantilla de Casos de Uso.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -163,9 +168,6 @@
     <t>Consultar grupos</t>
   </si>
   <si>
-    <t>Consultar proximos pagos</t>
-  </si>
-  <si>
     <t>CRU Alumno</t>
   </si>
   <si>
@@ -229,9 +231,6 @@
     <t xml:space="preserve">El profesor visualiza todos los pagos realizados correctamente por los alumnos </t>
   </si>
   <si>
-    <t>El usuario del sistema visualiza los pagos proximos a efectuarse ya sea de alumnos o de profesores</t>
-  </si>
-  <si>
     <t>El director debera poder administrar la informacion de los alumnos creando y modificando los registros</t>
   </si>
   <si>
@@ -296,12 +295,18 @@
   </si>
   <si>
     <t>El director podra administrar la informacion de un cliente que rente el espacio</t>
+  </si>
+  <si>
+    <t>El profesor visualiza los pagos proximos a efectuarse de los alumnos</t>
+  </si>
+  <si>
+    <t>Consultar proximos pagos de alumnos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -439,6 +444,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -732,7 +740,7 @@
   <dimension ref="B1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,10 +799,10 @@
         <v>23</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>37</v>
@@ -815,10 +823,10 @@
         <v>24</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>38</v>
@@ -839,7 +847,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>39</v>
@@ -863,10 +871,10 @@
         <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>38</v>
@@ -887,7 +895,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>42</v>
@@ -911,10 +919,10 @@
         <v>28</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>38</v>
@@ -935,7 +943,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>41</v>
@@ -959,7 +967,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>40</v>
@@ -983,10 +991,10 @@
         <v>31</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>38</v>
@@ -1007,10 +1015,10 @@
         <v>32</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>38</v>
@@ -1031,10 +1039,10 @@
         <v>33</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>38</v>
@@ -1055,10 +1063,10 @@
         <v>34</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>38</v>
@@ -1079,10 +1087,10 @@
         <v>35</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>38</v>
@@ -1103,10 +1111,10 @@
         <v>36</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>38</v>
@@ -1124,13 +1132,13 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>38</v>
@@ -1148,13 +1156,13 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>38</v>
@@ -1172,13 +1180,13 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>38</v>
@@ -1196,13 +1204,13 @@
     </row>
     <row r="22" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>38</v>
@@ -1220,13 +1228,13 @@
     </row>
     <row r="23" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>38</v>
@@ -1244,13 +1252,13 @@
     </row>
     <row r="24" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>38</v>
@@ -1268,13 +1276,13 @@
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
Corrección de casos de uso y plantilla de casos de uso.
Se modifican los casos de uso 16 y 17 CRU egreso y CRU gasto promocional
en descripciones, modelo de CU y plantilla de casos de uso.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla de Casos de Uso.xlsx
+++ b/Plantillas/Plantilla de Casos de Uso.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -19,7 +14,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Casos de Uso'!$A$1:$I$27</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$13</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="100">
   <si>
     <t>Columna</t>
   </si>
@@ -195,12 +190,6 @@
     <t>Generar reporte de ingresos y egresos</t>
   </si>
   <si>
-    <t>Registrar egreso</t>
-  </si>
-  <si>
-    <t>Registrar gasto promocional</t>
-  </si>
-  <si>
     <t>CRU promoción</t>
   </si>
   <si>
@@ -249,12 +238,6 @@
     <t>El director puede visualizar movimientos mensuales e imprimir un reporte general de todas las trasacciones.</t>
   </si>
   <si>
-    <t>El director puede registrar un gasto realizado</t>
-  </si>
-  <si>
-    <t>El director puede registrar un gasto de una promocion de facebook</t>
-  </si>
-  <si>
     <t>Cambiar alumno de grupo</t>
   </si>
   <si>
@@ -328,12 +311,33 @@
   </si>
   <si>
     <t>Consultar grupos y rentas</t>
+  </si>
+  <si>
+    <t>CRU egreso</t>
+  </si>
+  <si>
+    <t>CRU gasto promocional</t>
+  </si>
+  <si>
+    <t>El director puede administrar gastos de promociones de facebook</t>
+  </si>
+  <si>
+    <t>El director puede administrar gastos realizados</t>
+  </si>
+  <si>
+    <t>CU - 25</t>
+  </si>
+  <si>
+    <t>El director puede consultar cualquier tipo de gasto de la institución</t>
+  </si>
+  <si>
+    <t>Consultar gastos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -466,8 +470,36 @@
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -766,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,10 +858,10 @@
         <v>23</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>37</v>
@@ -850,10 +882,10 @@
         <v>24</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>38</v>
@@ -874,7 +906,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>39</v>
@@ -898,10 +930,10 @@
         <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>38</v>
@@ -922,7 +954,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>42</v>
@@ -946,10 +978,10 @@
         <v>28</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>38</v>
@@ -970,7 +1002,7 @@
         <v>29</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>41</v>
@@ -994,7 +1026,7 @@
         <v>30</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>40</v>
@@ -1018,10 +1050,10 @@
         <v>31</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>38</v>
@@ -1042,7 +1074,7 @@
         <v>32</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>43</v>
@@ -1066,10 +1098,10 @@
         <v>33</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>38</v>
@@ -1090,10 +1122,10 @@
         <v>34</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>38</v>
@@ -1114,10 +1146,10 @@
         <v>35</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>38</v>
@@ -1138,10 +1170,10 @@
         <v>36</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>38</v>
@@ -1162,10 +1194,10 @@
         <v>44</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>38</v>
@@ -1186,10 +1218,10 @@
         <v>45</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>38</v>
@@ -1210,10 +1242,10 @@
         <v>46</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>38</v>
@@ -1234,7 +1266,7 @@
         <v>47</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>51</v>
@@ -1258,10 +1290,10 @@
         <v>48</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>38</v>
@@ -1282,10 +1314,10 @@
         <v>49</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>38</v>
@@ -1306,10 +1338,10 @@
         <v>50</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>38</v>
@@ -1327,13 +1359,13 @@
     </row>
     <row r="26" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>38</v>
@@ -1351,13 +1383,13 @@
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>94</v>
-      </c>
       <c r="D27" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>38</v>
@@ -1375,13 +1407,13 @@
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>95</v>
-      </c>
       <c r="D28" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>38</v>
@@ -1398,13 +1430,27 @@
       <c r="I28" s="6"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
+      <c r="B29" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="6">
+        <v>0</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0</v>
+      </c>
+      <c r="H29" s="6">
+        <v>1</v>
+      </c>
       <c r="I29" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Diagramas de robustez y secuencia CU 03 y 04
se crean los diagramas de robustez y secuencia de los casos de uso consultar proximos pagos y generar recibo de pago
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla de Casos de Uso.xlsx
+++ b/Plantillas/Plantilla de Casos de Uso.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -14,7 +19,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Casos de Uso'!$A$1:$I$27</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$13</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -145,9 +150,6 @@
     <t>CU- 14</t>
   </si>
   <si>
-    <t>vacío</t>
-  </si>
-  <si>
     <t>vacio</t>
   </si>
   <si>
@@ -332,12 +334,15 @@
   </si>
   <si>
     <t>Consultar gastos</t>
+  </si>
+  <si>
+    <t>planificado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -798,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,16 +863,16 @@
         <v>23</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="F5" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G5" s="6">
         <v>0</v>
@@ -882,13 +887,13 @@
         <v>24</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" s="6">
         <v>0</v>
@@ -906,13 +911,13 @@
         <v>25</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" s="6">
         <v>0</v>
@@ -930,16 +935,16 @@
         <v>26</v>
       </c>
       <c r="C8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>82</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>38</v>
+        <v>99</v>
       </c>
       <c r="F8" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G8" s="6">
         <v>0</v>
@@ -954,13 +959,13 @@
         <v>27</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="6">
         <v>0</v>
@@ -978,13 +983,13 @@
         <v>28</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="6">
         <v>0</v>
@@ -1002,13 +1007,13 @@
         <v>29</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="6">
         <v>0</v>
@@ -1026,13 +1031,13 @@
         <v>30</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F12" s="6">
         <v>0</v>
@@ -1050,13 +1055,13 @@
         <v>31</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" s="6">
         <v>0</v>
@@ -1074,13 +1079,13 @@
         <v>32</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="6">
         <v>0</v>
@@ -1098,13 +1103,13 @@
         <v>33</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F15" s="6">
         <v>0</v>
@@ -1122,13 +1127,13 @@
         <v>34</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F16" s="6">
         <v>0</v>
@@ -1146,13 +1151,13 @@
         <v>35</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F17" s="6">
         <v>0</v>
@@ -1170,13 +1175,13 @@
         <v>36</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" s="6">
         <v>0</v>
@@ -1191,16 +1196,16 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F19" s="6">
         <v>0</v>
@@ -1215,16 +1220,16 @@
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20" s="6">
         <v>0</v>
@@ -1239,16 +1244,16 @@
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="6">
         <v>0</v>
@@ -1263,16 +1268,16 @@
     </row>
     <row r="22" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F22" s="6">
         <v>0</v>
@@ -1287,16 +1292,16 @@
     </row>
     <row r="23" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F23" s="6">
         <v>0</v>
@@ -1311,16 +1316,16 @@
     </row>
     <row r="24" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F24" s="6">
         <v>0</v>
@@ -1335,16 +1340,16 @@
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F25" s="6">
         <v>0</v>
@@ -1359,16 +1364,16 @@
     </row>
     <row r="26" spans="2:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="E26" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F26" s="6">
         <v>0</v>
@@ -1383,16 +1388,16 @@
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F27" s="6">
         <v>0</v>
@@ -1407,16 +1412,16 @@
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F28" s="6">
         <v>0</v>
@@ -1431,16 +1436,16 @@
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>99</v>
-      </c>
       <c r="E29" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F29" s="6">
         <v>0</v>

</xml_diff>

<commit_message>
Modulo de egresos caso de uso gasto promocional
Se implementa parciamente el caso de uso gasto promocional y
correcciones en casos de uso de iteracion anterior(sesiones)
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla de Casos de Uso.xlsx
+++ b/Plantillas/Plantilla de Casos de Uso.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B21E6623-E6CC-4DB3-AAD6-E1ADB347C8C5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -352,7 +346,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -510,7 +504,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -810,11 +804,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,10 +1233,10 @@
         <v>91</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="F20" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G20" s="6">
         <v>0</v>
@@ -1507,7 +1501,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C12"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="B6" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Plantilla de tareas de la 6ta iteración
Plantilla de tareas correspondiente a la 6ta iteración (parte del 90 %)
y actualización a la plantilla de casos de uso.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla de Casos de Uso.xlsx
+++ b/Plantillas/Plantilla de Casos de Uso.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{37EE53EB-C05F-4FFF-B053-931C1C38FA42}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF89CF7-2F1D-4D74-AC9C-70D8BC76C548}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Casos de Uso'!$A$1:$I$27</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$13</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,7 +1041,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="6">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H11" s="6">
         <v>1</v>
@@ -1065,7 +1065,7 @@
         <v>4</v>
       </c>
       <c r="G12" s="6">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H12" s="6">
         <v>1</v>
@@ -1329,7 +1329,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="6">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H23" s="6">
         <v>1</v>
@@ -1521,7 +1521,7 @@
         <v>2</v>
       </c>
       <c r="G31" s="6">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="H31" s="6">
         <v>1</v>

</xml_diff>

<commit_message>
Plantilla de tareas de la 7ma iteración.
Se agrega la plantilla de tareas de la 7ma iteración y la retrospectiva
de la 6ta.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla de Casos de Uso.xlsx
+++ b/Plantillas/Plantilla de Casos de Uso.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A20CE3C9-6AD6-4D03-B18B-B0194F566A52}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9573A0DE-0537-4097-B3EA-EDF913DDE567}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,7 +1323,7 @@
         <v>74</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F23" s="6">
         <v>7</v>

</xml_diff>